<commit_message>
!!!!!!all done!!!!!! # minor changes
</commit_message>
<xml_diff>
--- a/manual_save_test.xlsx
+++ b/manual_save_test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,216 +614,176 @@
       <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="B11" t="n">
-        <v>600</v>
-      </c>
-      <c r="C11" t="n">
-        <v>35</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>5</v>
-      </c>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RESV</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>9.300000000000001</v>
-      </c>
-      <c r="B12" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C12" t="n">
-        <v>40</v>
-      </c>
-      <c r="D12" t="n">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>p_e</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>r_e</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>k_r</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>k_z</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>18</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2500</v>
+      </c>
+      <c r="C13" t="n">
+        <v>50</v>
+      </c>
+      <c r="D13" t="n">
+        <v>20</v>
+      </c>
+      <c r="E13" t="n">
         <v>0.1</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F13" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="G13" t="n">
         <v>5</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>RESV</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>p_e</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>r_e</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>PHI</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>k_r</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>k_z</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>mu</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>18</v>
-      </c>
-      <c r="B15" t="n">
-        <v>2500</v>
-      </c>
-      <c r="C15" t="n">
-        <v>50</v>
-      </c>
-      <c r="D15" t="n">
-        <v>20</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="G15" t="n">
-        <v>5</v>
-      </c>
-      <c r="H15" t="n">
-        <v>1.25</v>
-      </c>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SKIN</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>well 1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>well 2</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>well 3</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>well 4</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>well 5</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>well 6</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>well 7</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>well 8</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>SKIN</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>well 1</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>well 2</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>well 3</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>well 4</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>well 5</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>well 6</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>well 7</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>well 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
+      <c r="A17" t="n">
         <v>13.39959646420044</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B17" t="n">
         <v>18.00233633067132</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C17" t="n">
         <v>23.92211863125592</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D17" t="n">
         <v>49.74479585300448</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E17" t="n">
         <v>16.66016394268236</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F17" t="n">
         <v>36.94554472880635</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G17" t="n">
         <v>22.4963334470802</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H17" t="n">
         <v>56.12788659134501</v>
       </c>
     </row>

</xml_diff>